<commit_message>
Atualizado documentação do projeto
</commit_message>
<xml_diff>
--- a/Docs/Produt_Backlog.xlsx
+++ b/Docs/Produt_Backlog.xlsx
@@ -13,15 +13,15 @@
   </definedNames>
   <calcPr/>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mg6/uX5ahPM3aGhswrCb2ccSSVwXw=="/>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="7g+I7oo7srZXExg7uq2QZddq4Vh6e/GKicb9R/lA8OU="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="34">
   <si>
     <t>Product Backlog Ágil</t>
   </si>
@@ -53,100 +53,61 @@
     <t>Sim</t>
   </si>
   <si>
-    <t>Não</t>
-  </si>
-  <si>
     <t>Alta</t>
   </si>
   <si>
-    <t>Em Progresso</t>
+    <t>Completa</t>
   </si>
   <si>
-    <t>Criar perfil de usuarios</t>
+    <t>1 - Criar perfil de Usuario</t>
+  </si>
+  <si>
+    <t>4 - Criar areas de plantação</t>
   </si>
   <si>
     <t>Média</t>
   </si>
   <si>
-    <t>Não Iniciada</t>
+    <t>6 - Cadastrar  Area total da plantação</t>
   </si>
   <si>
-    <t>Gerar cadastro para Usuários</t>
+    <t>7 - Cadastrar rotinas de irrigação</t>
   </si>
   <si>
-    <t>Criar relatórios de consumo (Água)</t>
+    <t>13 - Calcular o coeficiente de cultura</t>
   </si>
   <si>
     <t>Sprint 2</t>
   </si>
   <si>
-    <t>Criar relatórios de consumo (pesticida)</t>
+    <t>12 - Notificar ao Gestor quando uma nova rotina for cadastrada</t>
   </si>
   <si>
     <t>Baixa</t>
   </si>
   <si>
-    <t>Criar um sistema de rotinas</t>
+    <t>3 - Validar as Rotinas de Irrigação</t>
   </si>
   <si>
-    <t>Garantir que os usuários possam colocar os dados</t>
+    <t>8 - Editar rotinas de irrigação que não foram aprovadas</t>
+  </si>
+  <si>
+    <t>9 - Ativar Rotina de Irrigação</t>
   </si>
   <si>
     <t>Sprint 3</t>
   </si>
   <si>
-    <t>Validar as rotinas de irrigação no sistema</t>
+    <t>5 - Desativar Rotinas de Irrigação</t>
   </si>
   <si>
-    <t>Retribuir ao usuário um esquema de rotinas</t>
+    <t>11 - Notificar ao Gestor quando está saindo do periodo de alguma plantação</t>
   </si>
   <si>
-    <t>Criar relatórios sobre a plantação</t>
+    <t>2 - Extrair Relatórios de consumo  suprimentos</t>
   </si>
   <si>
-    <t>Sprint 4</t>
-  </si>
-  <si>
-    <t>Devolver ao usuário um relatório do produto final</t>
-  </si>
-  <si>
-    <t>Inserir dados sobre quantidade de água utilizada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verificação de funcionamento das rotinas </t>
-  </si>
-  <si>
-    <t>Inserir dados sobre o tipo de produto produzido</t>
-  </si>
-  <si>
-    <t>Sprint 5</t>
-  </si>
-  <si>
-    <t>Criar mapeamento da área</t>
-  </si>
-  <si>
-    <t>Automatizar processo de irrigação</t>
-  </si>
-  <si>
-    <t>Criar formulário para a área total do terreno e dividi-las em sessões</t>
-  </si>
-  <si>
-    <t>Criar relatórios sobre as áreas de irrigação</t>
-  </si>
-  <si>
-    <t>Sprint 6</t>
-  </si>
-  <si>
-    <t>Devolver ao usuário um relatório da área  definida</t>
-  </si>
-  <si>
-    <t>Garantir que o Gestor possa alterar possíveis erros</t>
-  </si>
-  <si>
-    <t>Crar sistema para gerenciar Rotinas</t>
-  </si>
-  <si>
-    <t>Criar sistema de notificação</t>
+    <t>10 - Executar rotinas de irrigação</t>
   </si>
   <si>
     <t>Crie um Product Backlog Ágil no Smartsheet</t>
@@ -155,14 +116,20 @@
     <t>Essa planilha permite construir a lista suspensa</t>
   </si>
   <si>
-    <t>Completa</t>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Em Progresso</t>
+  </si>
+  <si>
+    <t>Não Iniciada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -202,11 +169,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -240,7 +202,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border/>
     <border>
       <left/>
@@ -252,6 +214,17 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -294,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -306,39 +279,40 @@
     <xf borderId="2" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
+    <xf borderId="2" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="9" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="10" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -381,7 +355,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="16230600" cy="4657725"/>
@@ -654,7 +628,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -682,7 +656,7 @@
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -822,17 +796,16 @@
         <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="4">
-        <f>SUM(F8:F10)</f>
-        <v>40</v>
+      <c r="F7" s="5">
+        <v>31.0</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>9</v>
@@ -859,25 +832,25 @@
       <c r="AA7" s="1"/>
     </row>
     <row r="8" ht="21.75" customHeight="1">
-      <c r="A8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="6">
-        <v>16.0</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="E8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="7">
+        <v>6.0</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="1"/>
@@ -902,25 +875,25 @@
       <c r="AA8" s="1"/>
     </row>
     <row r="9" ht="21.75" customHeight="1">
-      <c r="A9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="6">
-        <v>8.0</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="E9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="1"/>
@@ -945,25 +918,25 @@
       <c r="AA9" s="1"/>
     </row>
     <row r="10" ht="21.75" customHeight="1">
-      <c r="A10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="A10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="6">
-        <v>16.0</v>
-      </c>
-      <c r="G10" s="6" t="s">
+      <c r="E10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="7">
+        <v>4.0</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="1"/>
@@ -988,27 +961,26 @@
       <c r="AA10" s="1"/>
     </row>
     <row r="11" ht="21.75" customHeight="1">
-      <c r="A11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="A11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="4">
-        <f>SUM(F12:F14)</f>
-        <v>96</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>10</v>
+      <c r="E11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="9">
+        <v>9.0</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1032,25 +1004,25 @@
       <c r="AA11" s="1"/>
     </row>
     <row r="12" ht="21.75" customHeight="1">
-      <c r="A12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="6">
-        <v>32.0</v>
-      </c>
-      <c r="G12" s="6" t="s">
+      <c r="A12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="11">
+        <v>7.0</v>
+      </c>
+      <c r="G12" s="11" t="s">
         <v>9</v>
       </c>
       <c r="H12" s="1"/>
@@ -1075,25 +1047,26 @@
       <c r="AA12" s="1"/>
     </row>
     <row r="13" ht="21.75" customHeight="1">
-      <c r="A13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="6">
-        <v>48.0</v>
-      </c>
-      <c r="G13" s="6" t="s">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="4">
+        <f>SUM(F14:F17)</f>
+        <v>25</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H13" s="1"/>
@@ -1118,26 +1091,26 @@
       <c r="AA13" s="1"/>
     </row>
     <row r="14" ht="21.75" customHeight="1">
-      <c r="A14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="6">
-        <v>16.0</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>10</v>
+      <c r="A14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="7">
+        <v>4.0</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1161,27 +1134,26 @@
       <c r="AA14" s="1"/>
     </row>
     <row r="15" ht="21.75" customHeight="1">
-      <c r="A15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="A15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="4">
-        <f>SUM(F16:F18)</f>
-        <v>32</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>10</v>
+      <c r="E15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="7">
+        <v>6.0</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1205,26 +1177,26 @@
       <c r="AA15" s="1"/>
     </row>
     <row r="16" ht="21.75" customHeight="1">
-      <c r="A16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="6">
-        <v>8.0</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>10</v>
+      <c r="A16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1248,26 +1220,26 @@
       <c r="AA16" s="1"/>
     </row>
     <row r="17" ht="21.75" customHeight="1">
-      <c r="A17" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="6">
-        <v>8.0</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>10</v>
+      <c r="E17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="7">
+        <v>10.0</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -1291,26 +1263,27 @@
       <c r="AA17" s="1"/>
     </row>
     <row r="18" ht="21.75" customHeight="1">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="4">
+        <f>SUM(F19:F22)</f>
         <v>26</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="6">
-        <v>16.0</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>10</v>
+      <c r="G18" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1334,27 +1307,26 @@
       <c r="AA18" s="1"/>
     </row>
     <row r="19" ht="21.75" customHeight="1">
-      <c r="A19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="A19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="4">
-        <f>SUM(F20:F23)</f>
-        <v>96</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>10</v>
+      <c r="E19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -1378,26 +1350,26 @@
       <c r="AA19" s="1"/>
     </row>
     <row r="20" ht="21.75" customHeight="1">
-      <c r="A20" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="6">
-        <v>32.0</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>10</v>
+      <c r="A20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="7">
+        <v>4.0</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -1421,26 +1393,26 @@
       <c r="AA20" s="1"/>
     </row>
     <row r="21" ht="21.75" customHeight="1">
-      <c r="A21" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="A21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="6">
-        <v>32.0</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>10</v>
+      <c r="E21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="7">
+        <v>8.0</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -1464,26 +1436,26 @@
       <c r="AA21" s="1"/>
     </row>
     <row r="22" ht="21.75" customHeight="1">
-      <c r="A22" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="6">
-        <v>32.0</v>
-      </c>
-      <c r="G22" s="6" t="s">
+      <c r="A22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>10</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="7">
+        <v>9.0</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1506,28 +1478,14 @@
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" ht="21.75" customHeight="1">
-      <c r="A23" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>10</v>
-      </c>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1549,29 +1507,14 @@
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" ht="21.75" customHeight="1">
-      <c r="A24" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="4">
-        <f>SUM(F25:F34)</f>
-        <v>216</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>10</v>
-      </c>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1593,34 +1536,22 @@
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
     </row>
-    <row r="25" ht="21.75" customHeight="1">
-      <c r="A25" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="6">
-        <v>48.0</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="15"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -1636,34 +1567,10 @@
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
     </row>
-    <row r="26" ht="21.75" customHeight="1">
-      <c r="A26" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="6">
-        <v>8.0</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="16"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="15"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -1679,34 +1586,10 @@
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
     </row>
-    <row r="27" ht="21.75" customHeight="1">
-      <c r="A27" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="6">
-        <v>8.0</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="16"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="15"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -1722,34 +1605,10 @@
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
     </row>
-    <row r="28" ht="21.75" customHeight="1">
-      <c r="A28" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="6">
-        <v>8.0</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="16"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="15"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -1765,35 +1624,10 @@
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
     </row>
-    <row r="29" ht="21.75" customHeight="1">
-      <c r="A29" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="4">
-        <f>SUM(F30:F39)</f>
-        <v>72</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="16"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="15"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
@@ -1809,34 +1643,20 @@
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
     </row>
-    <row r="30" ht="21.75" customHeight="1">
-      <c r="A30" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" s="6">
-        <v>32.0</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="18"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="15"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
@@ -1852,28 +1672,14 @@
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
     </row>
-    <row r="31" ht="21.75" customHeight="1">
-      <c r="A31" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="6">
-        <v>8.0</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>10</v>
-      </c>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -1895,28 +1701,14 @@
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
     </row>
-    <row r="32" ht="21.75" customHeight="1">
-      <c r="A32" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F32" s="6">
-        <v>16.0</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>10</v>
-      </c>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -1938,28 +1730,14 @@
       <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
     </row>
-    <row r="33" ht="21.75" customHeight="1">
-      <c r="A33" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33" s="6">
-        <v>16.0</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>10</v>
-      </c>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -1981,14 +1759,14 @@
       <c r="Z33" s="1"/>
       <c r="AA33" s="1"/>
     </row>
-    <row r="34" ht="21.75" customHeight="1">
-      <c r="A34" s="7"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -2069,21 +1847,19 @@
       <c r="AA36" s="1"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="14"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
@@ -2100,9 +1876,19 @@
       <c r="AA37" s="1"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="15"/>
-      <c r="L38" s="16"/>
-      <c r="M38" s="14"/>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
@@ -2119,9 +1905,19 @@
       <c r="AA38" s="1"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="15"/>
-      <c r="L39" s="16"/>
-      <c r="M39" s="14"/>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
@@ -2138,9 +1934,19 @@
       <c r="AA39" s="1"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="15"/>
-      <c r="L40" s="16"/>
-      <c r="M40" s="14"/>
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
@@ -2157,9 +1963,19 @@
       <c r="AA40" s="1"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="15"/>
-      <c r="L41" s="16"/>
-      <c r="M41" s="14"/>
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
@@ -2176,19 +1992,19 @@
       <c r="AA41" s="1"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="17"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18"/>
-      <c r="L42" s="19"/>
-      <c r="M42" s="14"/>
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
@@ -2958,354 +2774,18 @@
       <c r="Z68" s="1"/>
       <c r="AA68" s="1"/>
     </row>
-    <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
-      <c r="N69" s="1"/>
-      <c r="O69" s="1"/>
-      <c r="P69" s="1"/>
-      <c r="Q69" s="1"/>
-      <c r="R69" s="1"/>
-      <c r="S69" s="1"/>
-      <c r="T69" s="1"/>
-      <c r="U69" s="1"/>
-      <c r="V69" s="1"/>
-      <c r="W69" s="1"/>
-      <c r="X69" s="1"/>
-      <c r="Y69" s="1"/>
-      <c r="Z69" s="1"/>
-      <c r="AA69" s="1"/>
-    </row>
-    <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="P70" s="1"/>
-      <c r="Q70" s="1"/>
-      <c r="R70" s="1"/>
-      <c r="S70" s="1"/>
-      <c r="T70" s="1"/>
-      <c r="U70" s="1"/>
-      <c r="V70" s="1"/>
-      <c r="W70" s="1"/>
-      <c r="X70" s="1"/>
-      <c r="Y70" s="1"/>
-      <c r="Z70" s="1"/>
-      <c r="AA70" s="1"/>
-    </row>
-    <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
-      <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
-      <c r="N71" s="1"/>
-      <c r="O71" s="1"/>
-      <c r="P71" s="1"/>
-      <c r="Q71" s="1"/>
-      <c r="R71" s="1"/>
-      <c r="S71" s="1"/>
-      <c r="T71" s="1"/>
-      <c r="U71" s="1"/>
-      <c r="V71" s="1"/>
-      <c r="W71" s="1"/>
-      <c r="X71" s="1"/>
-      <c r="Y71" s="1"/>
-      <c r="Z71" s="1"/>
-      <c r="AA71" s="1"/>
-    </row>
-    <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-      <c r="L72" s="1"/>
-      <c r="M72" s="1"/>
-      <c r="N72" s="1"/>
-      <c r="O72" s="1"/>
-      <c r="P72" s="1"/>
-      <c r="Q72" s="1"/>
-      <c r="R72" s="1"/>
-      <c r="S72" s="1"/>
-      <c r="T72" s="1"/>
-      <c r="U72" s="1"/>
-      <c r="V72" s="1"/>
-      <c r="W72" s="1"/>
-      <c r="X72" s="1"/>
-      <c r="Y72" s="1"/>
-      <c r="Z72" s="1"/>
-      <c r="AA72" s="1"/>
-    </row>
-    <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-      <c r="L73" s="1"/>
-      <c r="M73" s="1"/>
-      <c r="N73" s="1"/>
-      <c r="O73" s="1"/>
-      <c r="P73" s="1"/>
-      <c r="Q73" s="1"/>
-      <c r="R73" s="1"/>
-      <c r="S73" s="1"/>
-      <c r="T73" s="1"/>
-      <c r="U73" s="1"/>
-      <c r="V73" s="1"/>
-      <c r="W73" s="1"/>
-      <c r="X73" s="1"/>
-      <c r="Y73" s="1"/>
-      <c r="Z73" s="1"/>
-      <c r="AA73" s="1"/>
-    </row>
-    <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
-      <c r="M74" s="1"/>
-      <c r="N74" s="1"/>
-      <c r="O74" s="1"/>
-      <c r="P74" s="1"/>
-      <c r="Q74" s="1"/>
-      <c r="R74" s="1"/>
-      <c r="S74" s="1"/>
-      <c r="T74" s="1"/>
-      <c r="U74" s="1"/>
-      <c r="V74" s="1"/>
-      <c r="W74" s="1"/>
-      <c r="X74" s="1"/>
-      <c r="Y74" s="1"/>
-      <c r="Z74" s="1"/>
-      <c r="AA74" s="1"/>
-    </row>
-    <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="1"/>
-      <c r="K75" s="1"/>
-      <c r="L75" s="1"/>
-      <c r="M75" s="1"/>
-      <c r="N75" s="1"/>
-      <c r="O75" s="1"/>
-      <c r="P75" s="1"/>
-      <c r="Q75" s="1"/>
-      <c r="R75" s="1"/>
-      <c r="S75" s="1"/>
-      <c r="T75" s="1"/>
-      <c r="U75" s="1"/>
-      <c r="V75" s="1"/>
-      <c r="W75" s="1"/>
-      <c r="X75" s="1"/>
-      <c r="Y75" s="1"/>
-      <c r="Z75" s="1"/>
-      <c r="AA75" s="1"/>
-    </row>
-    <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
-      <c r="L76" s="1"/>
-      <c r="M76" s="1"/>
-      <c r="N76" s="1"/>
-      <c r="O76" s="1"/>
-      <c r="P76" s="1"/>
-      <c r="Q76" s="1"/>
-      <c r="R76" s="1"/>
-      <c r="S76" s="1"/>
-      <c r="T76" s="1"/>
-      <c r="U76" s="1"/>
-      <c r="V76" s="1"/>
-      <c r="W76" s="1"/>
-      <c r="X76" s="1"/>
-      <c r="Y76" s="1"/>
-      <c r="Z76" s="1"/>
-      <c r="AA76" s="1"/>
-    </row>
-    <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
-      <c r="L77" s="1"/>
-      <c r="M77" s="1"/>
-      <c r="N77" s="1"/>
-      <c r="O77" s="1"/>
-      <c r="P77" s="1"/>
-      <c r="Q77" s="1"/>
-      <c r="R77" s="1"/>
-      <c r="S77" s="1"/>
-      <c r="T77" s="1"/>
-      <c r="U77" s="1"/>
-      <c r="V77" s="1"/>
-      <c r="W77" s="1"/>
-      <c r="X77" s="1"/>
-      <c r="Y77" s="1"/>
-      <c r="Z77" s="1"/>
-      <c r="AA77" s="1"/>
-    </row>
-    <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
-      <c r="H78" s="1"/>
-      <c r="I78" s="1"/>
-      <c r="J78" s="1"/>
-      <c r="K78" s="1"/>
-      <c r="L78" s="1"/>
-      <c r="M78" s="1"/>
-      <c r="N78" s="1"/>
-      <c r="O78" s="1"/>
-      <c r="P78" s="1"/>
-      <c r="Q78" s="1"/>
-      <c r="R78" s="1"/>
-      <c r="S78" s="1"/>
-      <c r="T78" s="1"/>
-      <c r="U78" s="1"/>
-      <c r="V78" s="1"/>
-      <c r="W78" s="1"/>
-      <c r="X78" s="1"/>
-      <c r="Y78" s="1"/>
-      <c r="Z78" s="1"/>
-      <c r="AA78" s="1"/>
-    </row>
-    <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
-      <c r="I79" s="1"/>
-      <c r="J79" s="1"/>
-      <c r="K79" s="1"/>
-      <c r="L79" s="1"/>
-      <c r="M79" s="1"/>
-      <c r="N79" s="1"/>
-      <c r="O79" s="1"/>
-      <c r="P79" s="1"/>
-      <c r="Q79" s="1"/>
-      <c r="R79" s="1"/>
-      <c r="S79" s="1"/>
-      <c r="T79" s="1"/>
-      <c r="U79" s="1"/>
-      <c r="V79" s="1"/>
-      <c r="W79" s="1"/>
-      <c r="X79" s="1"/>
-      <c r="Y79" s="1"/>
-      <c r="Z79" s="1"/>
-      <c r="AA79" s="1"/>
-    </row>
-    <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
-      <c r="J80" s="1"/>
-      <c r="K80" s="1"/>
-      <c r="L80" s="1"/>
-      <c r="M80" s="1"/>
-      <c r="N80" s="1"/>
-      <c r="O80" s="1"/>
-      <c r="P80" s="1"/>
-      <c r="Q80" s="1"/>
-      <c r="R80" s="1"/>
-      <c r="S80" s="1"/>
-      <c r="T80" s="1"/>
-      <c r="U80" s="1"/>
-      <c r="V80" s="1"/>
-      <c r="W80" s="1"/>
-      <c r="X80" s="1"/>
-      <c r="Y80" s="1"/>
-      <c r="Z80" s="1"/>
-      <c r="AA80" s="1"/>
-    </row>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="70" ht="15.75" customHeight="1"/>
+    <row r="71" ht="15.75" customHeight="1"/>
+    <row r="72" ht="15.75" customHeight="1"/>
+    <row r="73" ht="15.75" customHeight="1"/>
+    <row r="74" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1"/>
+    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1"/>
+    <row r="78" ht="15.75" customHeight="1"/>
+    <row r="79" ht="15.75" customHeight="1"/>
+    <row r="80" ht="15.75" customHeight="1"/>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1"/>
     <row r="83" ht="15.75" customHeight="1"/>
@@ -4220,31 +3700,19 @@
     <row r="992" ht="15.75" customHeight="1"/>
     <row r="993" ht="15.75" customHeight="1"/>
     <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
-    <row r="1001" ht="15.75" customHeight="1"/>
-    <row r="1002" ht="15.75" customHeight="1"/>
-    <row r="1003" ht="15.75" customHeight="1"/>
-    <row r="1004" ht="15.75" customHeight="1"/>
-    <row r="1005" ht="15.75" customHeight="1"/>
-    <row r="1006" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A37:L42"/>
+    <mergeCell ref="A25:L30"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E7:E34">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E7:E22">
       <formula1>Status</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D7:D34">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B7:C22 G7:G22">
+      <formula1>YesNo</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D7:D22">
       <formula1>Priority</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B7:C34 G7:G34">
-      <formula1>YesNo</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions/>
@@ -4263,47 +3731,44 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="6" width="11.22"/>
-  </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1"/>
     <row r="2" ht="15.75" customHeight="1"/>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="20" t="s">
-        <v>43</v>
+      <c r="A3" s="21" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1"/>
     <row r="5" ht="15.75" customHeight="1"/>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="21" t="s">
+      <c r="A6" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="21" t="s">
+      <c r="A7" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>12</v>
+      <c r="C7" s="22" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>15</v>
+      <c r="C8" s="22" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1"/>

</xml_diff>